<commit_message>
Adicionado content description no layout e corrigido erros de execucao
</commit_message>
<xml_diff>
--- a/documentos/ListaMatrial.xlsx
+++ b/documentos/ListaMatrial.xlsx
@@ -111,7 +111,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -196,48 +196,79 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -521,151 +552,165 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="10"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="5"/>
     </row>
     <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="13"/>
+      <c r="A2" s="6"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="8"/>
     </row>
     <row r="3" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3" t="s">
+      <c r="B3" s="12"/>
+      <c r="C3" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3" t="s">
+      <c r="D3" s="12"/>
+      <c r="E3" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3" t="s">
+      <c r="F3" s="12"/>
+      <c r="G3" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="3"/>
+      <c r="H3" s="12"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5">
+      <c r="B4" s="10"/>
+      <c r="C4" s="10">
         <v>5</v>
       </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="6">
+      <c r="D4" s="10"/>
+      <c r="E4" s="13">
         <v>41.03</v>
       </c>
-      <c r="F4" s="5"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="15"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5">
+      <c r="B5" s="10"/>
+      <c r="C5" s="10">
         <v>1</v>
       </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="6">
+      <c r="D5" s="10"/>
+      <c r="E5" s="13">
         <v>10</v>
       </c>
-      <c r="F5" s="5"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="15"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5">
+      <c r="B6" s="10"/>
+      <c r="C6" s="10">
         <v>2</v>
       </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="15"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5">
+      <c r="B7" s="10"/>
+      <c r="C7" s="10">
         <v>2</v>
       </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="15"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5">
+      <c r="B8" s="10"/>
+      <c r="C8" s="10">
         <v>1</v>
       </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="15"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5">
+      <c r="B9" s="10"/>
+      <c r="C9" s="10">
         <v>1</v>
       </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="15"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J13" s="14"/>
+      <c r="J13" s="2"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I14" s="2"/>
+      <c r="I14" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="24">
+  <mergeCells count="30">
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:D3"/>
     <mergeCell ref="A1:H2"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="C6:D6"/>
@@ -682,14 +727,6 @@
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E4:F4"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>